<commit_message>
Created indirect solution method and low level heuristics
</commit_message>
<xml_diff>
--- a/V1/Dataset/GECCO19.xlsx
+++ b/V1/Dataset/GECCO19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pylya\Desktop\PhD\PhD\github\CSPLib\V1\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147F2B26-D46C-4262-955D-6C210BC15497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0003F713-2837-4ECB-9270-7E0F4723938A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="900" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="22" r:id="rId1"/>
@@ -1737,7 +1737,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="644">
   <si>
     <t>Sessions</t>
   </si>
@@ -3574,9 +3574,6 @@
     <t>person128</t>
   </si>
   <si>
-    <t>person30, person34, person62. person79, person148, person129</t>
-  </si>
-  <si>
     <t>person180, person130</t>
   </si>
   <si>
@@ -3857,6 +3854,243 @@
   </si>
   <si>
     <t>Forum Hall</t>
+  </si>
+  <si>
+    <t>person2</t>
+  </si>
+  <si>
+    <t>person6</t>
+  </si>
+  <si>
+    <t>person10</t>
+  </si>
+  <si>
+    <t>person12</t>
+  </si>
+  <si>
+    <t>person13</t>
+  </si>
+  <si>
+    <t>person15</t>
+  </si>
+  <si>
+    <t>person18</t>
+  </si>
+  <si>
+    <t>person20</t>
+  </si>
+  <si>
+    <t>person32</t>
+  </si>
+  <si>
+    <t>person35</t>
+  </si>
+  <si>
+    <t>person36</t>
+  </si>
+  <si>
+    <t>person37</t>
+  </si>
+  <si>
+    <t>person38</t>
+  </si>
+  <si>
+    <t>person41</t>
+  </si>
+  <si>
+    <t>person42</t>
+  </si>
+  <si>
+    <t>person45</t>
+  </si>
+  <si>
+    <t>person47</t>
+  </si>
+  <si>
+    <t>person51</t>
+  </si>
+  <si>
+    <t>person52</t>
+  </si>
+  <si>
+    <t>person55</t>
+  </si>
+  <si>
+    <t>person56</t>
+  </si>
+  <si>
+    <t>person57</t>
+  </si>
+  <si>
+    <t>person58</t>
+  </si>
+  <si>
+    <t>person60</t>
+  </si>
+  <si>
+    <t>person62</t>
+  </si>
+  <si>
+    <t>person64</t>
+  </si>
+  <si>
+    <t>person65</t>
+  </si>
+  <si>
+    <t>person67</t>
+  </si>
+  <si>
+    <t>person68</t>
+  </si>
+  <si>
+    <t>person70</t>
+  </si>
+  <si>
+    <t>person72</t>
+  </si>
+  <si>
+    <t>person75</t>
+  </si>
+  <si>
+    <t>person77</t>
+  </si>
+  <si>
+    <t>person78</t>
+  </si>
+  <si>
+    <t>person80</t>
+  </si>
+  <si>
+    <t>person81</t>
+  </si>
+  <si>
+    <t>person82</t>
+  </si>
+  <si>
+    <t>person83</t>
+  </si>
+  <si>
+    <t>person85</t>
+  </si>
+  <si>
+    <t>person87</t>
+  </si>
+  <si>
+    <t>person92</t>
+  </si>
+  <si>
+    <t>person93</t>
+  </si>
+  <si>
+    <t>person94</t>
+  </si>
+  <si>
+    <t>person95</t>
+  </si>
+  <si>
+    <t>person100</t>
+  </si>
+  <si>
+    <t>person105</t>
+  </si>
+  <si>
+    <t>person107</t>
+  </si>
+  <si>
+    <t>person113</t>
+  </si>
+  <si>
+    <t>person115</t>
+  </si>
+  <si>
+    <t>person117</t>
+  </si>
+  <si>
+    <t>person118</t>
+  </si>
+  <si>
+    <t>person122</t>
+  </si>
+  <si>
+    <t>person123</t>
+  </si>
+  <si>
+    <t>person126</t>
+  </si>
+  <si>
+    <t>person129</t>
+  </si>
+  <si>
+    <t>person130</t>
+  </si>
+  <si>
+    <t>person131</t>
+  </si>
+  <si>
+    <t>person133</t>
+  </si>
+  <si>
+    <t>person134</t>
+  </si>
+  <si>
+    <t>person135</t>
+  </si>
+  <si>
+    <t>person143</t>
+  </si>
+  <si>
+    <t>person155</t>
+  </si>
+  <si>
+    <t>person158</t>
+  </si>
+  <si>
+    <t>person163</t>
+  </si>
+  <si>
+    <t>person164</t>
+  </si>
+  <si>
+    <t>person165</t>
+  </si>
+  <si>
+    <t>person169</t>
+  </si>
+  <si>
+    <t>person170</t>
+  </si>
+  <si>
+    <t>person173</t>
+  </si>
+  <si>
+    <t>person177</t>
+  </si>
+  <si>
+    <t>person178</t>
+  </si>
+  <si>
+    <t>person182</t>
+  </si>
+  <si>
+    <t>person186</t>
+  </si>
+  <si>
+    <t>person188</t>
+  </si>
+  <si>
+    <t>person189</t>
+  </si>
+  <si>
+    <t>person190</t>
+  </si>
+  <si>
+    <t>person194</t>
+  </si>
+  <si>
+    <t>person195</t>
+  </si>
+  <si>
+    <t>person30, person34, person62, person79, person148, person129</t>
   </si>
 </sst>
 </file>
@@ -4165,17 +4399,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4186,6 +4411,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4194,12 +4425,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4213,10 +4438,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4233,9 +4470,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4258,17 +4492,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4563,143 +4797,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="50"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="51"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="51"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="50"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="32" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="52"/>
@@ -4786,221 +5020,221 @@
       <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="59"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="59"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="59"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="61"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="42"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="60"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="60"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="61"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="60"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="61"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="42"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="42"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="60"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="61"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="42"/>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="40"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="41"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="37"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="34"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="34"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="31"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="34"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="31"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="33"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="34"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="40"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="41"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="37"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="37"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="36"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="43"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="40"/>
     </row>
     <row r="52" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="31"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="60"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="46"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="47"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="46"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="47"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="31"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="60"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="31"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="60"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="27" t="s">
@@ -5009,427 +5243,439 @@
       <c r="E57" s="18"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="31"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="31"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="39"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="44"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="38"/>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="39"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="44"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="38"/>
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="39"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="44"/>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="41"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="36"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="36"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="37"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="36"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="42" t="s">
+      <c r="A66" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="42"/>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="43"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="40"/>
     </row>
     <row r="67" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="31"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="60"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="29"/>
+      <c r="A68" s="45"/>
+      <c r="B68" s="45"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="46"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="37"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="36"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="36"/>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="37"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="36"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="38" t="s">
+      <c r="A71" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="39"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="44"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="38"/>
-      <c r="B72" s="38"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="39"/>
+      <c r="A72" s="43"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="44"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="38"/>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="39"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="38"/>
-      <c r="B74" s="38"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="39"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="44"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="38"/>
-      <c r="B75" s="38"/>
-      <c r="C75" s="38"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="39"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="44"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="38"/>
-      <c r="B76" s="38"/>
-      <c r="C76" s="38"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="39"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+      <c r="E76" s="44"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="38"/>
-      <c r="B77" s="38"/>
-      <c r="C77" s="38"/>
-      <c r="D77" s="38"/>
-      <c r="E77" s="39"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+      <c r="E77" s="44"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="38"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="39"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="43"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="44"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="44"/>
-      <c r="B79" s="44"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="45"/>
+      <c r="A79" s="61"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="62"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="35" t="s">
+      <c r="A80" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="37"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="36"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="37"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="36"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="38" t="s">
+      <c r="A82" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="38"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="39"/>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="44"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="38"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="39"/>
+      <c r="A83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="44"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="38"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="39"/>
+      <c r="A84" s="43"/>
+      <c r="B84" s="43"/>
+      <c r="C84" s="43"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="44"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="38"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="39"/>
+      <c r="A85" s="43"/>
+      <c r="B85" s="43"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="44"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="38"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="39"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="44"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" s="38"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="39"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="43"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="44"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="38"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="39"/>
+      <c r="A88" s="43"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="44"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="38"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="39"/>
+      <c r="A89" s="43"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="44"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="29"/>
+      <c r="A90" s="45"/>
+      <c r="B90" s="45"/>
+      <c r="C90" s="45"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="46"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="35" t="s">
+      <c r="A91" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="37"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="36"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="36"/>
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="37"/>
+      <c r="A92" s="35"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="36"/>
     </row>
     <row r="93" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="38" t="s">
+      <c r="A93" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B93" s="38"/>
-      <c r="C93" s="38"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="39"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="44"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="38"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="39"/>
+      <c r="A94" s="43"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+      <c r="D94" s="43"/>
+      <c r="E94" s="44"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="38"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="38"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="39"/>
+      <c r="A95" s="43"/>
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+      <c r="D95" s="43"/>
+      <c r="E95" s="44"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="38"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="39"/>
+      <c r="A96" s="43"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="43"/>
+      <c r="D96" s="43"/>
+      <c r="E96" s="44"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="38"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="38"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="39"/>
+      <c r="A97" s="43"/>
+      <c r="B97" s="43"/>
+      <c r="C97" s="43"/>
+      <c r="D97" s="43"/>
+      <c r="E97" s="44"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="38"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="38"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="39"/>
+      <c r="A98" s="43"/>
+      <c r="B98" s="43"/>
+      <c r="C98" s="43"/>
+      <c r="D98" s="43"/>
+      <c r="E98" s="44"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="38"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="38"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="39"/>
+      <c r="A99" s="43"/>
+      <c r="B99" s="43"/>
+      <c r="C99" s="43"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="44"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="38"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="38"/>
-      <c r="D100" s="38"/>
-      <c r="E100" s="39"/>
+      <c r="A100" s="43"/>
+      <c r="B100" s="43"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+      <c r="E100" s="44"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" s="28"/>
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="29"/>
+      <c r="A101" s="45"/>
+      <c r="B101" s="45"/>
+      <c r="C101" s="45"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="46"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="35" t="s">
+      <c r="A102" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B102" s="36"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="37"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="36"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="37"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="36"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="38" t="s">
+      <c r="A104" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B104" s="38"/>
-      <c r="C104" s="38"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="39"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="44"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="38"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="38"/>
-      <c r="D105" s="38"/>
-      <c r="E105" s="39"/>
+      <c r="A105" s="43"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="44"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="38"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="39"/>
+      <c r="A106" s="43"/>
+      <c r="B106" s="43"/>
+      <c r="C106" s="43"/>
+      <c r="D106" s="43"/>
+      <c r="E106" s="44"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="38"/>
-      <c r="B107" s="38"/>
-      <c r="C107" s="38"/>
-      <c r="D107" s="38"/>
-      <c r="E107" s="39"/>
+      <c r="A107" s="43"/>
+      <c r="B107" s="43"/>
+      <c r="C107" s="43"/>
+      <c r="D107" s="43"/>
+      <c r="E107" s="44"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="38"/>
-      <c r="B108" s="38"/>
-      <c r="C108" s="38"/>
-      <c r="D108" s="38"/>
-      <c r="E108" s="39"/>
+      <c r="A108" s="43"/>
+      <c r="B108" s="43"/>
+      <c r="C108" s="43"/>
+      <c r="D108" s="43"/>
+      <c r="E108" s="44"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="38"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="38"/>
-      <c r="D109" s="38"/>
-      <c r="E109" s="39"/>
+      <c r="A109" s="43"/>
+      <c r="B109" s="43"/>
+      <c r="C109" s="43"/>
+      <c r="D109" s="43"/>
+      <c r="E109" s="44"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="38"/>
-      <c r="B110" s="38"/>
-      <c r="C110" s="38"/>
-      <c r="D110" s="38"/>
-      <c r="E110" s="39"/>
+      <c r="A110" s="43"/>
+      <c r="B110" s="43"/>
+      <c r="C110" s="43"/>
+      <c r="D110" s="43"/>
+      <c r="E110" s="44"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="38"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="38"/>
-      <c r="D111" s="38"/>
-      <c r="E111" s="39"/>
+      <c r="A111" s="43"/>
+      <c r="B111" s="43"/>
+      <c r="C111" s="43"/>
+      <c r="D111" s="43"/>
+      <c r="E111" s="44"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="28"/>
-      <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="29"/>
+      <c r="A112" s="45"/>
+      <c r="B112" s="45"/>
+      <c r="C112" s="45"/>
+      <c r="D112" s="45"/>
+      <c r="E112" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A44:E45"/>
-    <mergeCell ref="A46:E47"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A41:E42"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E39"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A58:E59"/>
+    <mergeCell ref="A91:E92"/>
+    <mergeCell ref="A93:E100"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A69:E70"/>
+    <mergeCell ref="A60:E62"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A64:E65"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A71:E78"/>
+    <mergeCell ref="A102:E103"/>
+    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A79:E79"/>
     <mergeCell ref="A80:E81"/>
     <mergeCell ref="A82:E89"/>
     <mergeCell ref="A90:E90"/>
@@ -5446,27 +5692,15 @@
     <mergeCell ref="A20:E21"/>
     <mergeCell ref="A55:E55"/>
     <mergeCell ref="A27:E29"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A58:E59"/>
-    <mergeCell ref="A91:E92"/>
-    <mergeCell ref="A93:E100"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="A69:E70"/>
-    <mergeCell ref="A60:E62"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A64:E65"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A71:E78"/>
-    <mergeCell ref="A102:E103"/>
-    <mergeCell ref="A104:E111"/>
+    <mergeCell ref="A44:E45"/>
+    <mergeCell ref="A46:E47"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A41:E42"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6218,7 +6452,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
@@ -6233,34 +6467,34 @@
     <row r="1" spans="1:24" s="3" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -6278,57 +6512,57 @@
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -6655,9 +6889,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I128" sqref="I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6710,37 +6944,37 @@
         <v>5</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>544</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>545</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>547</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>549</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="U1" s="16" t="s">
         <v>553</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>554</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>555</v>
       </c>
       <c r="W1" s="16" t="s">
         <v>47</v>
@@ -6748,35 +6982,35 @@
       <c r="X1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="62" t="s">
+      <c r="Y1" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="Z1" s="28" t="s">
         <v>556</v>
       </c>
-      <c r="Z1" s="62" t="s">
+      <c r="AA1" s="28" t="s">
         <v>557</v>
       </c>
-      <c r="AA1" s="62" t="s">
+      <c r="AB1" s="28" t="s">
         <v>558</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AC1" s="28" t="s">
         <v>559</v>
       </c>
-      <c r="AC1" s="62" t="s">
+      <c r="AD1" s="28" t="s">
         <v>560</v>
       </c>
-      <c r="AD1" s="62" t="s">
+      <c r="AE1" s="28" t="s">
         <v>561</v>
       </c>
-      <c r="AE1" s="62" t="s">
+      <c r="AF1" s="28" t="s">
         <v>562</v>
       </c>
-      <c r="AF1" s="62" t="s">
+      <c r="AG1" s="28" t="s">
         <v>563</v>
       </c>
-      <c r="AG1" s="62" t="s">
+      <c r="AH1" s="28" t="s">
         <v>564</v>
-      </c>
-      <c r="AH1" s="62" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10485,7 +10719,7 @@
         <v>1</v>
       </c>
       <c r="J130" s="9" t="s">
-        <v>471</v>
+        <v>643</v>
       </c>
       <c r="M130" s="9"/>
       <c r="Z130" s="1"/>
@@ -10513,7 +10747,7 @@
         <v>1</v>
       </c>
       <c r="J131" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Z131" s="1"/>
     </row>
@@ -10540,7 +10774,7 @@
         <v>1</v>
       </c>
       <c r="J132" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Z132" s="1"/>
     </row>
@@ -10567,7 +10801,7 @@
         <v>1</v>
       </c>
       <c r="J133" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Z133" s="1"/>
     </row>
@@ -10594,7 +10828,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="135" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10620,7 +10854,7 @@
         <v>1</v>
       </c>
       <c r="J135" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="136" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10646,7 +10880,7 @@
         <v>1</v>
       </c>
       <c r="J136" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="137" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10672,7 +10906,7 @@
         <v>1</v>
       </c>
       <c r="J137" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="138" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10698,7 +10932,7 @@
         <v>1</v>
       </c>
       <c r="J138" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="139" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10724,7 +10958,7 @@
         <v>1</v>
       </c>
       <c r="J139" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="140" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10750,7 +10984,7 @@
         <v>1</v>
       </c>
       <c r="J140" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10776,7 +11010,7 @@
         <v>1</v>
       </c>
       <c r="J141" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="142" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10802,7 +11036,7 @@
         <v>1</v>
       </c>
       <c r="J142" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="143" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10828,7 +11062,7 @@
         <v>1</v>
       </c>
       <c r="J143" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="144" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -10854,7 +11088,7 @@
         <v>1</v>
       </c>
       <c r="J144" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="L144" s="9"/>
     </row>
@@ -10883,7 +11117,7 @@
       <c r="H145" s="11"/>
       <c r="I145" s="11"/>
       <c r="J145" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K145" s="6"/>
       <c r="L145" s="1"/>
@@ -10925,7 +11159,7 @@
       <c r="H146" s="11"/>
       <c r="I146" s="11"/>
       <c r="J146" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K146" s="6"/>
       <c r="L146" s="1"/>
@@ -10967,7 +11201,7 @@
       <c r="H147" s="11"/>
       <c r="I147" s="11"/>
       <c r="J147" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K147" s="6"/>
       <c r="L147" s="1"/>
@@ -11009,7 +11243,7 @@
       <c r="H148" s="11"/>
       <c r="I148" s="11"/>
       <c r="J148" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K148" s="6"/>
       <c r="L148" s="1"/>
@@ -11051,7 +11285,7 @@
       <c r="H149" s="11"/>
       <c r="I149" s="11"/>
       <c r="J149" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K149" s="6"/>
       <c r="L149" s="1"/>
@@ -11093,7 +11327,7 @@
       <c r="H150" s="11"/>
       <c r="I150" s="11"/>
       <c r="J150" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K150" s="6"/>
       <c r="L150" s="1"/>
@@ -11135,7 +11369,7 @@
       <c r="H151" s="11"/>
       <c r="I151" s="11"/>
       <c r="J151" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K151" s="6"/>
       <c r="L151" s="1"/>
@@ -11177,7 +11411,7 @@
       <c r="H152" s="11"/>
       <c r="I152" s="11"/>
       <c r="J152" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K152" s="6"/>
       <c r="L152" s="1"/>
@@ -11219,7 +11453,7 @@
       <c r="H153" s="11"/>
       <c r="I153" s="11"/>
       <c r="J153" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K153" s="6"/>
       <c r="L153" s="1"/>
@@ -11261,7 +11495,7 @@
       <c r="H154" s="11"/>
       <c r="I154" s="11"/>
       <c r="J154" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K154" s="6"/>
       <c r="L154" s="1"/>
@@ -11303,7 +11537,7 @@
       <c r="H155" s="11"/>
       <c r="I155" s="11"/>
       <c r="J155" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K155" s="6"/>
       <c r="L155" s="1"/>
@@ -11345,7 +11579,7 @@
       <c r="H156" s="11"/>
       <c r="I156" s="11"/>
       <c r="J156" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K156" s="6"/>
       <c r="L156" s="1"/>
@@ -11387,7 +11621,7 @@
       <c r="H157" s="11"/>
       <c r="I157" s="11"/>
       <c r="J157" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="K157" s="6"/>
       <c r="L157" s="1"/>
@@ -11427,7 +11661,7 @@
         <v>1</v>
       </c>
       <c r="J158" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="159" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11453,7 +11687,7 @@
         <v>1</v>
       </c>
       <c r="J159" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="160" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11479,7 +11713,7 @@
         <v>1</v>
       </c>
       <c r="J160" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="161" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11505,7 +11739,7 @@
         <v>1</v>
       </c>
       <c r="J161" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11531,7 +11765,7 @@
         <v>1</v>
       </c>
       <c r="J162" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11557,7 +11791,7 @@
         <v>1</v>
       </c>
       <c r="J163" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11583,7 +11817,7 @@
         <v>1</v>
       </c>
       <c r="J164" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="165" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11609,7 +11843,7 @@
         <v>1</v>
       </c>
       <c r="J165" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11635,7 +11869,7 @@
         <v>1</v>
       </c>
       <c r="J166" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="167" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11661,7 +11895,7 @@
         <v>1</v>
       </c>
       <c r="J167" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="168" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11687,7 +11921,7 @@
         <v>1</v>
       </c>
       <c r="J168" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11713,7 +11947,7 @@
         <v>1</v>
       </c>
       <c r="J169" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11739,7 +11973,7 @@
         <v>1</v>
       </c>
       <c r="J170" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11765,7 +11999,7 @@
         <v>1</v>
       </c>
       <c r="J171" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11791,7 +12025,7 @@
         <v>1</v>
       </c>
       <c r="J172" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11817,7 +12051,7 @@
         <v>1</v>
       </c>
       <c r="J173" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11843,7 +12077,7 @@
         <v>1</v>
       </c>
       <c r="J174" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11869,7 +12103,7 @@
         <v>1</v>
       </c>
       <c r="J175" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="176" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11895,7 +12129,7 @@
         <v>1</v>
       </c>
       <c r="J176" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="177" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11921,7 +12155,7 @@
         <v>1</v>
       </c>
       <c r="J177" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="178" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11947,7 +12181,7 @@
         <v>1</v>
       </c>
       <c r="J178" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="179" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11973,7 +12207,7 @@
         <v>1</v>
       </c>
       <c r="J179" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="180" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -11999,7 +12233,7 @@
         <v>1</v>
       </c>
       <c r="J180" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="181" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12025,7 +12259,7 @@
         <v>1</v>
       </c>
       <c r="J181" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="182" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12051,7 +12285,7 @@
         <v>1</v>
       </c>
       <c r="J182" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="183" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12077,7 +12311,7 @@
         <v>1</v>
       </c>
       <c r="J183" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="184" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12103,7 +12337,7 @@
         <v>1</v>
       </c>
       <c r="J184" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="185" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12129,7 +12363,7 @@
         <v>1</v>
       </c>
       <c r="J185" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="186" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12155,7 +12389,7 @@
         <v>1</v>
       </c>
       <c r="J186" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="187" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12181,7 +12415,7 @@
         <v>1</v>
       </c>
       <c r="J187" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="188" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12207,7 +12441,7 @@
         <v>1</v>
       </c>
       <c r="J188" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="189" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12233,7 +12467,7 @@
         <v>1</v>
       </c>
       <c r="J189" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12259,7 +12493,7 @@
         <v>1</v>
       </c>
       <c r="J190" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="191" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12285,7 +12519,7 @@
         <v>1</v>
       </c>
       <c r="J191" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="192" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12311,7 +12545,7 @@
         <v>1</v>
       </c>
       <c r="J192" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="193" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12337,7 +12571,7 @@
         <v>1</v>
       </c>
       <c r="J193" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="194" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12363,7 +12597,7 @@
         <v>1</v>
       </c>
       <c r="J194" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="195" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12389,7 +12623,7 @@
         <v>1</v>
       </c>
       <c r="J195" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="196" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12415,7 +12649,7 @@
         <v>1</v>
       </c>
       <c r="J196" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="197" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12441,7 +12675,7 @@
         <v>1</v>
       </c>
       <c r="J197" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="198" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12467,7 +12701,7 @@
         <v>1</v>
       </c>
       <c r="J198" s="9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M198" s="1">
         <v>1</v>
@@ -12529,7 +12763,7 @@
         <v>1</v>
       </c>
       <c r="J199" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="L199" s="1">
         <v>1</v>
@@ -12591,7 +12825,7 @@
         <v>1</v>
       </c>
       <c r="J200" s="9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L200" s="1">
         <v>1</v>
@@ -12653,7 +12887,7 @@
         <v>1</v>
       </c>
       <c r="J201" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="202" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12679,7 +12913,7 @@
         <v>1</v>
       </c>
       <c r="J202" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="203" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12705,7 +12939,7 @@
         <v>1</v>
       </c>
       <c r="J203" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -13234,10 +13468,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CFC106-4249-4BC9-9967-425037A65B0D}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13280,160 +13514,1672 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>343</v>
+      </c>
       <c r="H2" s="6"/>
+      <c r="I2" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>565</v>
+      </c>
       <c r="H3" s="6"/>
+      <c r="I3" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>345</v>
+      </c>
       <c r="H4" s="6"/>
+      <c r="I4" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>346</v>
+      </c>
       <c r="H5" s="6"/>
+      <c r="I5" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>347</v>
+      </c>
       <c r="H6" s="6"/>
+      <c r="I6" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>566</v>
+      </c>
       <c r="H7" s="6"/>
+      <c r="I7" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>349</v>
+      </c>
       <c r="H8" s="6"/>
+      <c r="I8" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>350</v>
+      </c>
       <c r="H9" s="6"/>
+      <c r="I9" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>351</v>
+      </c>
       <c r="H10" s="6"/>
+      <c r="I10" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>567</v>
+      </c>
       <c r="H11" s="6"/>
+      <c r="I11" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="H12" s="6"/>
+      <c r="I12" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>568</v>
+      </c>
       <c r="H13" s="6"/>
+      <c r="I13" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>569</v>
+      </c>
       <c r="H14" s="6"/>
+      <c r="I14" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>356</v>
+      </c>
       <c r="H15" s="6"/>
+      <c r="I15" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>570</v>
+      </c>
       <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>358</v>
+      </c>
       <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>359</v>
+      </c>
       <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>571</v>
+      </c>
       <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>361</v>
+      </c>
       <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>572</v>
+      </c>
       <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>363</v>
+      </c>
       <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>364</v>
+      </c>
       <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>365</v>
+      </c>
       <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>366</v>
+      </c>
       <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>367</v>
+      </c>
       <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>368</v>
+      </c>
       <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>369</v>
+      </c>
       <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>370</v>
+      </c>
       <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>371</v>
+      </c>
       <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>372</v>
+      </c>
       <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>373</v>
+      </c>
       <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>573</v>
+      </c>
       <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>375</v>
+      </c>
       <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>376</v>
+      </c>
       <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>574</v>
+      </c>
       <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>575</v>
+      </c>
       <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>576</v>
+      </c>
       <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>577</v>
+      </c>
       <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>381</v>
+      </c>
       <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>382</v>
+      </c>
       <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>578</v>
+      </c>
       <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>579</v>
+      </c>
       <c r="H43" s="6"/>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>385</v>
+      </c>
       <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>580</v>
+      </c>
       <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>388</v>
+      </c>
       <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I47" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>581</v>
+      </c>
       <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I48" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>390</v>
+      </c>
       <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I49" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>391</v>
+      </c>
       <c r="H50" s="6"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I50" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>392</v>
+      </c>
       <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I51" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>582</v>
+      </c>
       <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="I52" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>583</v>
+      </c>
       <c r="H53" s="6"/>
+      <c r="I53" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="I54" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="I55" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="I56" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="I57" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="I58" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="I59" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="I60" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="I61" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="I62" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="I63" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="I64" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="I65" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="I66" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="I67" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="I68" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="I69" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="I70" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="I71" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="I72" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="I73" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="I74" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="I75" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="I76" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="I77" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="I78" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="I79" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="I80" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="I81" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="I82" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="I83" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="I84" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I85" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="I86" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="I87" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="I88" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="I89" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="I90" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="I91" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="I92" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="I93" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="I94" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="I95" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="I96" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="I97" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="I98" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="I99" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="I100" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="I101" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="I102" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="I103" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="I104" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I105" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="I106" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="I107" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="I108" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="I109" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="I110" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="I111" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="I112" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="I113" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="I114" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="I115" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="I116" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="I117" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="I118" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="I119" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="I120" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="I121" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="I122" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="I123" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="I124" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="I125" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="I126" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="I127" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="I128" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="I129" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="I130" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="I131" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="I132" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="I133" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="I134" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="I135" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="I136" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A137" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="I137" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="I138" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="I139" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I140" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="I141" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="I142" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="I143" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="I144" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="I145" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="I146" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="I147" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="I148" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="I149" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="I150" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="I151" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="I152" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="I153" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="I154" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="I155" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A156" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="I156" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A157" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="I157" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="I158" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="I159" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="I160" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A161" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I161" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A162" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="I162" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="I163" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A164" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="I164" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="I165" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A166" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="I166" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="I167" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="I168" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="I169" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="I170" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="I171" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="I172" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="I173" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="I174" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="I175" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="I176" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="I177" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="I178" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="I179" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="I180" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="I181" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="I182" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A183" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="I183" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A184" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="I184" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A185" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="I185" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A186" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="I186" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="I187" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A188" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="I188" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="I189" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A190" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="I190" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A191" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="I191" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A192" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="I192" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="I193" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A194" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I194" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A195" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="I195" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="I196" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="I197" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A198" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I198" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A199" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="I199" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A200" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="I200" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="I201" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A202" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="I202" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="I203" s="9" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -13499,7 +15245,7 @@
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -13522,7 +15268,7 @@
     </row>
     <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>
@@ -13545,7 +15291,7 @@
     </row>
     <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -13568,7 +15314,7 @@
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -13591,7 +15337,7 @@
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -13614,7 +15360,7 @@
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B7" s="1">
         <v>4</v>
@@ -13637,7 +15383,7 @@
     </row>
     <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -13660,7 +15406,7 @@
     </row>
     <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -13683,7 +15429,7 @@
     </row>
     <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -13706,7 +15452,7 @@
     </row>
     <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -13729,7 +15475,7 @@
     </row>
     <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -13844,7 +15590,7 @@
     </row>
     <row r="2" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>88</v>
@@ -13852,7 +15598,7 @@
     </row>
     <row r="3" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>88</v>
@@ -13860,7 +15606,7 @@
     </row>
     <row r="4" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>88</v>
@@ -13868,7 +15614,7 @@
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>88</v>
@@ -13876,7 +15622,7 @@
     </row>
     <row r="6" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>88</v>
@@ -13884,7 +15630,7 @@
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>88</v>
@@ -13892,7 +15638,7 @@
     </row>
     <row r="8" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>88</v>
@@ -13900,7 +15646,7 @@
     </row>
     <row r="9" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>88</v>
@@ -13908,7 +15654,7 @@
     </row>
     <row r="10" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>88</v>
@@ -13916,7 +15662,7 @@
     </row>
     <row r="11" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>88</v>
@@ -13970,37 +15716,37 @@
     <row r="1" spans="1:14" s="3" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>554</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>555</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>47</v>
@@ -14760,34 +16506,34 @@
     <row r="1" spans="1:24" s="3" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>565</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>

</xml_diff>